<commit_message>
chest rewards, data streamlining
</commit_message>
<xml_diff>
--- a/data/chest_id.xlsx
+++ b/data/chest_id.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick McMahon\Dropbox\Emulators\FFV\FFV Hacking\CT_Hacking\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick McMahon\Dropbox\Emulators\FFV\FFV Hacking\CT_Hacking\FFVCareerDay\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873F20C7-2885-46C4-A70E-9B950AD8C546}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE263CBD-FE75-46EE-A47F-DB012BBA7E48}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14175" xr2:uid="{52CE9500-507D-4EBC-AA66-708E00F53115}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
   <si>
     <t>Chest</t>
   </si>
@@ -118,6 +118,18 @@
   </si>
   <si>
     <t>chest_name</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>Ability</t>
   </si>
 </sst>
 </file>
@@ -470,9 +482,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99FE56DA-46E6-401B-BF40-45B2DCD5E7D0}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -687,6 +701,22 @@
         <v>3</v>
       </c>
     </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>